<commit_message>
QA updates to the US Core IG
</commit_message>
<xml_diff>
--- a/input/images/tables/scopes.xlsx
+++ b/input/images/tables/scopes.xlsx
@@ -1328,7 +1328,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/3.1.0/CodeSystem-observation-category.html|social-history</t>
+          <t>http://terminology.hl7.org//CodeSystem-observation-category.html|social-history</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/3.1.0/CodeSystem-observation-category.html|social-history</t>
+          <t>http://terminology.hl7.org//CodeSystem-observation-category.html|social-history</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -1402,7 +1402,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/3.1.0/CodeSystem-observation-category.html|social-history</t>
+          <t>http://terminology.hl7.org//CodeSystem-observation-category.html|social-history</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/3.1.0/CodeSystem-observation-category.html|social-history</t>
+          <t>http://terminology.hl7.org//CodeSystem-observation-category.html|social-history</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
@@ -1719,7 +1719,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>http://terminology.hl7.org/3.1.0/CodeSystem-observation-category.html|social-history</t>
+          <t>http://terminology.hl7.org//CodeSystem-observation-category.html|social-history</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>

</xml_diff>